<commit_message>
Filled missing info in xlsx file
</commit_message>
<xml_diff>
--- a/data/mushrooms.xlsx
+++ b/data/mushrooms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maurice/repos_github/mushroom-identifier/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F6BE7E-108B-2E4A-9F88-370812E68168}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACADB4E8-94B9-934A-B4F2-E3576B148DDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28420" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="274">
   <si>
     <t>description</t>
   </si>
@@ -55,12 +55,6 @@
     <t>ntsam_cat</t>
   </si>
   <si>
-    <t>reig de fageda / reig bord</t>
-  </si>
-  <si>
-    <t>Not Poisonous</t>
-  </si>
-  <si>
     <t>Edible</t>
   </si>
   <si>
@@ -88,9 +82,6 @@
     <t>ntsbc_cat</t>
   </si>
   <si>
-    <t>Mataparent amarg</t>
-  </si>
-  <si>
     <t>ntsbe_cat</t>
   </si>
   <si>
@@ -124,9 +115,6 @@
     <t>ntsccos_cat</t>
   </si>
   <si>
-    <t>Cama-sec de bosc</t>
-  </si>
-  <si>
     <t>ntscco_cat</t>
   </si>
   <si>
@@ -175,9 +163,6 @@
     <t>ntsls_cat</t>
   </si>
   <si>
-    <t>Rovello</t>
-  </si>
-  <si>
     <t>ntslsu_cat</t>
   </si>
   <si>
@@ -214,9 +199,6 @@
     <t>Mataparent, Matagent</t>
   </si>
   <si>
-    <t>Poisonous</t>
-  </si>
-  <si>
     <t>ntssv_cat</t>
   </si>
   <si>
@@ -700,9 +682,6 @@
     <t>http://www.fichasmicologicas.com/?micos=1&amp;s=Melanoleuca%20Excissa&amp;art=439</t>
   </si>
   <si>
-    <t>OU DEL DIABLE</t>
-  </si>
-  <si>
     <t>http://www.fichasmicologicas.com/?micos=1&amp;s=Phallus%20Impudicus&amp;art=156</t>
   </si>
   <si>
@@ -715,9 +694,6 @@
     <t>http://www.fichasmicologicas.com/?micos=1&amp;s=Russula%20Cyanoxantha&amp;art=237</t>
   </si>
   <si>
-    <t>CARBONERA</t>
-  </si>
-  <si>
     <t>CARBONERA. SETA DE LOS CERDOS. URRETXA, URRITZ (Eusk.). PUABRA, CUALBRA, LLORA, PALOMINS, CAMADOLÇA, TERNADOLÇA (Cat.). CARBOEIRA (G.). BOLET DE CARBO (Val.)</t>
   </si>
   <si>
@@ -727,18 +703,12 @@
     <t>RÚSULA BLANCA. GIBELZURI ORRIZABAL (Eusk.). PEBRÁS, PEBRASSA BLANCA (Cat.). NETORRA BRANCA (G.). PEBRAÇ (Val.)</t>
   </si>
   <si>
-    <t>PEBRASSA BLANCA</t>
-  </si>
-  <si>
     <t>http://www.fichasmicologicas.com/?micos=1&amp;s=Russula%20Virescens&amp;art=255</t>
   </si>
   <si>
     <t>SETA DE CURA. GORRO VERDE. PALOMETA GIBELURDIN, URDINA, KOROSO (Eusk.). CUALBRA LLORA, LLORA VERDA(Cat.). FUNGO DOS CREGOS (G.). BOLET DE RETOR (Val.).</t>
   </si>
   <si>
-    <t>LLORA VERDA</t>
-  </si>
-  <si>
     <t>Sparassis_Crispa</t>
   </si>
   <si>
@@ -751,9 +721,6 @@
     <t>SETA EN FORMA DE COLIFLOR. CLAVARIA RIZADA. AZALORE BELAKI (Eusk.). PEU DE RATA REINA (Cat.). COUVEFLOR DO MONTE (G.)</t>
   </si>
   <si>
-    <t xml:space="preserve">PEU DE RATA REINA </t>
-  </si>
-  <si>
     <t>http://www.fichasmicologicas.com/?micos=1&amp;s=Suillus%20Variegatus&amp;art=1028</t>
   </si>
   <si>
@@ -775,15 +742,9 @@
     <t>http://www.fichasmicologicas.com/?micos=1&amp;s=Tricholoma&amp;art=186</t>
   </si>
   <si>
-    <t>Toxic</t>
-  </si>
-  <si>
     <t>TRICOLOMA AZUFRADO, OLOR A GAS. KIRATS ZIZA-HORI (Eusk.). GROGUET PUDENT (Cat.). TORTULLO CENDRADO (G.). BOLET DE SOFRE</t>
   </si>
   <si>
-    <t>BOLET DE SOFRE</t>
-  </si>
-  <si>
     <t>http://www.fichasmicologicas.com/?micos=1&amp;s=Tricholoma%20Terreum&amp;art=187</t>
   </si>
   <si>
@@ -818,6 +779,72 @@
   </si>
   <si>
     <t>Males imatges</t>
+  </si>
+  <si>
+    <t>Carbonera</t>
+  </si>
+  <si>
+    <t>Pebrassa Blanca</t>
+  </si>
+  <si>
+    <t>Llora Verda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peu de Rata Reina </t>
+  </si>
+  <si>
+    <t>Bolet de Sofre</t>
+  </si>
+  <si>
+    <t>Ou del Diable</t>
+  </si>
+  <si>
+    <t>Reig de Fageda, Reig Bord</t>
+  </si>
+  <si>
+    <t>Mataparent Amarg</t>
+  </si>
+  <si>
+    <t>Cama-Sec de Bosc</t>
+  </si>
+  <si>
+    <t>No. Edible</t>
+  </si>
+  <si>
+    <t>No. Edible with caution</t>
+  </si>
+  <si>
+    <t>No. Not Edible.</t>
+  </si>
+  <si>
+    <t>Yes.</t>
+  </si>
+  <si>
+    <t>Not poisonous.</t>
+  </si>
+  <si>
+    <t>No. Edible.</t>
+  </si>
+  <si>
+    <t>Pentinella</t>
+  </si>
+  <si>
+    <t>Sureny fosc, Cep negre</t>
+  </si>
+  <si>
+    <t>Bolet de Llop</t>
+  </si>
+  <si>
+    <t>Potsa de Perdiu</t>
+  </si>
+  <si>
+    <t>Puagra Retgera</t>
+  </si>
+  <si>
+    <t>Verderol, Grojet</t>
+  </si>
+  <si>
+    <t>Rovelló</t>
   </si>
 </sst>
 </file>
@@ -1331,7 +1358,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1356,6 +1383,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1714,8 +1744,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1733,10 +1766,10 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -1768,27 +1801,27 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1796,37 +1829,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
@@ -1836,17 +1869,17 @@
         <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>10</v>
+        <v>258</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="I4" s="3" t="s">
-        <v>11</v>
+      <c r="I4" s="10" t="s">
+        <v>263</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1854,27 +1887,27 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>63</v>
+        <v>264</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1882,27 +1915,27 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="3" t="s">
-        <v>63</v>
+      <c r="I6" s="10" t="s">
+        <v>264</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1910,25 +1943,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1936,53 +1969,53 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="H8" s="3"/>
-      <c r="I8" s="3" t="s">
-        <v>15</v>
+      <c r="I8" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>21</v>
+        <v>259</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7" t="s">
-        <v>11</v>
+        <v>263</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1990,27 +2023,27 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H10" s="3"/>
-      <c r="I10" s="3" t="s">
-        <v>15</v>
+      <c r="I10" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2018,25 +2051,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2044,25 +2077,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="H12" s="3"/>
-      <c r="I12" s="3" t="s">
-        <v>15</v>
+      <c r="I12" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2070,27 +2103,27 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2098,27 +2131,27 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H14" s="3"/>
-      <c r="I14" s="3" t="s">
-        <v>15</v>
+      <c r="I14" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2126,27 +2159,27 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2154,33 +2187,33 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="H16" s="3"/>
-      <c r="I16" s="3" t="s">
-        <v>15</v>
+      <c r="I16" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
@@ -2188,47 +2221,47 @@
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7" t="s">
-        <v>15</v>
+        <v>263</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H18" s="3"/>
-      <c r="I18" s="3" t="s">
-        <v>15</v>
+      <c r="I18" s="10" t="s">
+        <v>263</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -2236,29 +2269,29 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>33</v>
+        <v>260</v>
       </c>
       <c r="H19" s="7"/>
       <c r="I19" s="7" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="68" x14ac:dyDescent="0.2">
@@ -2266,27 +2299,27 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>15</v>
+        <v>243</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -2294,27 +2327,27 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7" t="s">
-        <v>11</v>
+        <v>266</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2322,7 +2355,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
@@ -2330,17 +2363,17 @@
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="H22" s="3"/>
-      <c r="I22" s="3" t="s">
-        <v>63</v>
+      <c r="I22" s="10" t="s">
+        <v>264</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2348,27 +2381,27 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="7" t="s">
-        <v>63</v>
+        <v>264</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2376,29 +2409,29 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H24" s="3"/>
-      <c r="I24" s="3" t="s">
-        <v>15</v>
+      <c r="I24" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2406,27 +2439,27 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="51" x14ac:dyDescent="0.2">
@@ -2434,27 +2467,27 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>15</v>
+        <v>199</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>261</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2462,7 +2495,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
@@ -2470,17 +2503,17 @@
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="7" t="s">
-        <v>63</v>
+        <v>264</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2488,25 +2521,25 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="H28" s="3"/>
-      <c r="I28" s="3" t="s">
-        <v>15</v>
+      <c r="I28" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2514,7 +2547,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7" t="s">
@@ -2522,17 +2555,17 @@
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2540,27 +2573,27 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H30" s="3"/>
-      <c r="I30" s="3" t="s">
-        <v>15</v>
+      <c r="I30" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -2568,29 +2601,29 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="7" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2598,27 +2631,27 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H32" s="3"/>
-      <c r="I32" s="3" t="s">
-        <v>15</v>
+      <c r="I32" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2626,25 +2659,25 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2652,25 +2685,25 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="H34" s="3"/>
-      <c r="I34" s="3" t="s">
-        <v>15</v>
+      <c r="I34" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2678,27 +2711,27 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="7" t="s">
-        <v>11</v>
+        <v>266</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2706,27 +2739,27 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H36" s="3"/>
-      <c r="I36" s="3" t="s">
-        <v>11</v>
+      <c r="I36" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2734,27 +2767,27 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>50</v>
+        <v>273</v>
       </c>
       <c r="H37" s="7"/>
       <c r="I37" s="7" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J37" s="8" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2762,23 +2795,23 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="3" t="s">
-        <v>15</v>
+      <c r="I38" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2786,27 +2819,27 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H39" s="7"/>
       <c r="I39" s="7" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2814,27 +2847,27 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H40" s="3"/>
-      <c r="I40" s="3" t="s">
-        <v>15</v>
+      <c r="I40" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="9" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -2842,113 +2875,113 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>11</v>
+        <v>266</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H42" s="3"/>
-      <c r="I42" s="3" t="s">
-        <v>15</v>
+      <c r="I42" s="10" t="s">
+        <v>265</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H43" s="7"/>
       <c r="I43" s="7" t="s">
-        <v>15</v>
+        <v>265</v>
       </c>
       <c r="J43" s="8" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H44" s="3"/>
-      <c r="I44" s="3" t="s">
-        <v>15</v>
+      <c r="I44" s="10" t="s">
+        <v>265</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2956,7 +2989,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="7" t="s">
@@ -2964,17 +2997,17 @@
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>225</v>
+        <v>257</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="7" t="s">
-        <v>63</v>
+        <v>264</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -2982,7 +3015,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
@@ -2990,271 +3023,271 @@
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="H46" s="3"/>
-      <c r="I46" s="3" t="s">
-        <v>63</v>
+      <c r="I46" s="10" t="s">
+        <v>264</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="4">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H47" s="7"/>
       <c r="I47" s="7" t="s">
-        <v>63</v>
+        <v>264</v>
       </c>
       <c r="J47" s="8" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="6">
+      <c r="A48" s="4">
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="H48" s="3"/>
-      <c r="I48" s="3" t="s">
-        <v>15</v>
+      <c r="I48" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A49" s="4">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="9" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A49" s="6">
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E49" s="7"/>
       <c r="F49" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J49" s="8" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A50" s="6">
+      <c r="A50" s="4">
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="I50" s="3"/>
+        <v>225</v>
+      </c>
+      <c r="I50" s="10"/>
       <c r="J50" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="4">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="7" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E51" s="7"/>
       <c r="F51" s="7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="7" t="s">
-        <v>220</v>
+        <v>264</v>
       </c>
       <c r="J51" s="8" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A52" s="6">
+      <c r="A52" s="4">
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>237</v>
+        <v>254</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>15</v>
+        <v>227</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A53" s="4">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A53" s="6">
         <v>52</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E53" s="7"/>
       <c r="F53" s="7" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J53" s="8" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A54" s="6">
+      <c r="A54" s="4">
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>15</v>
+        <v>233</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="4">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A55" s="6">
         <v>54</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="7" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E55" s="7"/>
       <c r="F55" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="H55" s="7"/>
       <c r="I55" s="7" t="s">
-        <v>15</v>
+        <v>262</v>
       </c>
       <c r="J55" s="8" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A56" s="6">
+      <c r="A56" s="4">
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
@@ -3262,52 +3295,53 @@
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>250</v>
+        <v>239</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>264</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
         <v>56</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="J57" s="8" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="4"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -3315,7 +3349,7 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
+      <c r="I58" s="10"/>
       <c r="J58" s="5"/>
     </row>
   </sheetData>

</xml_diff>